<commit_message>
add data test files
</commit_message>
<xml_diff>
--- a/data/Initial-World-Test1.xlsx
+++ b/data/Initial-World-Test1.xlsx
@@ -744,7 +744,7 @@
         </is>
       </c>
       <c r="E1" t="n">
-        <v>1.118043052837573</v>
+        <v>0.8834590401531538</v>
       </c>
       <c r="G1" t="inlineStr">
         <is>
@@ -812,26 +812,26 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Brobdingnag</t>
+          <t>Atlantis</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C3" t="n">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="D3" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
@@ -846,17 +846,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Dinotopia</t>
+          <t>Brobdingnag</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D4" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -865,7 +865,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -880,17 +880,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Erewhon</t>
+          <t>Carpania</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C5" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -899,7 +899,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -914,26 +914,26 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Atlantis</t>
+          <t>Dinotopia</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="D6" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
         <v>5</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>11</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -948,17 +948,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Carpania</t>
+          <t>Erewhon</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C7" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -967,7 +967,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -994,7 +994,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.8645142857142859</v>
+        <v>0.7739278245618743</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -1062,26 +1062,26 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Brobdingnag</t>
+          <t>Atlantis</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="D11" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H11" t="n">
         <v>2</v>
@@ -1096,17 +1096,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Dinotopia</t>
+          <t>Brobdingnag</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D12" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -1115,7 +1115,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1130,17 +1130,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Erewhon</t>
+          <t>Carpania</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C13" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D13" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -1149,7 +1149,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1164,26 +1164,26 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Atlantis</t>
+          <t>Dinotopia</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="D14" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
         <v>5</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" t="n">
-        <v>11</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1198,17 +1198,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Carpania</t>
+          <t>Erewhon</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C15" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D15" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -1217,7 +1217,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1244,7 +1244,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0.5783801652892564</v>
+        <v>0.6716430855176108</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1312,26 +1312,26 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Brobdingnag</t>
+          <t>Atlantis</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C19" t="n">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="D19" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H19" t="n">
         <v>3</v>
@@ -1346,17 +1346,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Dinotopia</t>
+          <t>Brobdingnag</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C20" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D20" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -1365,7 +1365,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
@@ -1380,17 +1380,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Erewhon</t>
+          <t>Carpania</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C21" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D21" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -1399,7 +1399,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -1414,26 +1414,26 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Atlantis</t>
+          <t>Dinotopia</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C22" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="D22" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
         <v>5</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" t="n">
-        <v>11</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -1448,17 +1448,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Carpania</t>
+          <t>Erewhon</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C23" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D23" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -1467,7 +1467,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -1494,7 +1494,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0.3733381294964029</v>
+        <v>0.5766048230203634</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1562,26 +1562,26 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Brobdingnag</t>
+          <t>Atlantis</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C27" t="n">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="D27" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H27" t="n">
         <v>4</v>
@@ -1596,17 +1596,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Dinotopia</t>
+          <t>Brobdingnag</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D28" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
@@ -1615,7 +1615,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
@@ -1630,17 +1630,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Erewhon</t>
+          <t>Carpania</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C29" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D29" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
@@ -1649,7 +1649,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
@@ -1664,26 +1664,26 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Atlantis</t>
+          <t>Dinotopia</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C30" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="D30" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
         <v>5</v>
-      </c>
-      <c r="F30" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" t="n">
-        <v>11</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -1698,17 +1698,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Carpania</t>
+          <t>Erewhon</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C31" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D31" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
@@ -1717,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -1744,7 +1744,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>0.2325095541401274</v>
+        <v>0.4888130370701321</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1812,26 +1812,26 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Brobdingnag</t>
+          <t>Atlantis</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C35" t="n">
+        <v>60</v>
+      </c>
+      <c r="D35" t="n">
         <v>20</v>
       </c>
-      <c r="D35" t="n">
-        <v>12</v>
-      </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H35" t="n">
         <v>5</v>
@@ -1846,17 +1846,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Dinotopia</t>
+          <t>Brobdingnag</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C36" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D36" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
@@ -1865,7 +1865,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
@@ -1880,17 +1880,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Erewhon</t>
+          <t>Carpania</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C37" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D37" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
@@ -1899,7 +1899,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
@@ -1914,26 +1914,26 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Atlantis</t>
+          <t>Dinotopia</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C38" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="D38" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
         <v>5</v>
-      </c>
-      <c r="F38" t="n">
-        <v>0</v>
-      </c>
-      <c r="G38" t="n">
-        <v>11</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
@@ -1948,17 +1948,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Carpania</t>
+          <t>Erewhon</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C39" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D39" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
@@ -1967,7 +1967,7 @@
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
@@ -1994,7 +1994,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>1.273916211293261</v>
+        <v>0.3873984592055312</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -2003,7 +2003,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>alloy_transform (in=[1.0, 2.0] out=[1.0, 1.0, 1.0]) (bins=1)</t>
+          <t>alloy_transform (in=[6.0, 12.0] out=[6.0, 6.0, 6.0]) (bins=6)</t>
         </is>
       </c>
     </row>
@@ -2062,29 +2062,29 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Brobdingnag</t>
+          <t>Atlantis</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C43" t="n">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="D43" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H43" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I43" t="n">
         <v>0</v>
@@ -2096,29 +2096,29 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Dinotopia</t>
+          <t>Brobdingnag</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C44" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D44" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" t="n">
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44" t="n">
         <v>0</v>
@@ -2130,17 +2130,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Erewhon</t>
+          <t>Carpania</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C45" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D45" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
@@ -2149,7 +2149,7 @@
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
@@ -2164,26 +2164,26 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Atlantis</t>
+          <t>Dinotopia</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C46" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="D46" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
         <v>5</v>
-      </c>
-      <c r="F46" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46" t="n">
-        <v>11</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
@@ -2198,17 +2198,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Carpania</t>
+          <t>Erewhon</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C47" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D47" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E47" t="n">
         <v>0</v>
@@ -2217,7 +2217,7 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
@@ -2244,7 +2244,7 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>0.8054144144144146</v>
+        <v>0.2911532482517948</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>alloy_transform (in=[2.0, 4.0] out=[2.0, 2.0, 2.0]) (bins=2)</t>
+          <t>alloy_transform (in=[7.0, 14.0] out=[7.0, 7.0, 7.0]) (bins=7)</t>
         </is>
       </c>
     </row>
@@ -2312,29 +2312,29 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Brobdingnag</t>
+          <t>Atlantis</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C51" t="n">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="D51" t="n">
+        <v>20</v>
+      </c>
+      <c r="E51" t="n">
         <v>12</v>
       </c>
-      <c r="E51" t="n">
-        <v>0</v>
-      </c>
       <c r="F51" t="n">
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H51" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I51" t="n">
         <v>0</v>
@@ -2346,29 +2346,29 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Dinotopia</t>
+          <t>Brobdingnag</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C52" t="n">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D52" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F52" t="n">
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H52" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I52" t="n">
         <v>0</v>
@@ -2380,17 +2380,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Erewhon</t>
+          <t>Carpania</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C53" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D53" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E53" t="n">
         <v>0</v>
@@ -2399,7 +2399,7 @@
         <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -2414,26 +2414,26 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Atlantis</t>
+          <t>Dinotopia</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C54" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="D54" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E54" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="n">
         <v>5</v>
-      </c>
-      <c r="F54" t="n">
-        <v>0</v>
-      </c>
-      <c r="G54" t="n">
-        <v>11</v>
       </c>
       <c r="H54" t="n">
         <v>0</v>
@@ -2448,17 +2448,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Carpania</t>
+          <t>Erewhon</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C55" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D55" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
@@ -2467,7 +2467,7 @@
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -2494,7 +2494,7 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>0.334506666666667</v>
+        <v>0.2156318289522959</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2503,7 +2503,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>alloy_transform (in=[3.0, 6.0] out=[3.0, 3.0, 3.0]) (bins=3)</t>
+          <t>alloy_transform (in=[8.0, 16.0] out=[8.0, 8.0, 8.0]) (bins=8)</t>
         </is>
       </c>
     </row>
@@ -2562,29 +2562,29 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Brobdingnag</t>
+          <t>Atlantis</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C59" t="n">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="D59" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E59" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F59" t="n">
         <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H59" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I59" t="n">
         <v>0</v>
@@ -2596,29 +2596,29 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Dinotopia</t>
+          <t>Brobdingnag</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C60" t="n">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D60" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F60" t="n">
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H60" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I60" t="n">
         <v>0</v>
@@ -2630,17 +2630,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Erewhon</t>
+          <t>Carpania</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C61" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D61" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E61" t="n">
         <v>0</v>
@@ -2649,7 +2649,7 @@
         <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H61" t="n">
         <v>0</v>
@@ -2664,26 +2664,26 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Atlantis</t>
+          <t>Dinotopia</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C62" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="D62" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E62" t="n">
+        <v>0</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" t="n">
         <v>5</v>
-      </c>
-      <c r="F62" t="n">
-        <v>0</v>
-      </c>
-      <c r="G62" t="n">
-        <v>11</v>
       </c>
       <c r="H62" t="n">
         <v>0</v>
@@ -2698,17 +2698,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Carpania</t>
+          <t>Erewhon</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C63" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D63" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E63" t="n">
         <v>0</v>
@@ -2717,7 +2717,7 @@
         <v>0</v>
       </c>
       <c r="G63" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
@@ -2744,7 +2744,7 @@
         </is>
       </c>
       <c r="E65" t="n">
-        <v>1.266083802439351</v>
+        <v>0.156363822814376</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2753,7 +2753,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>alloy_transform (in=[1.0, 2.0] out=[1.0, 1.0, 1.0]) (bins=1)</t>
+          <t>alloy_transform (in=[9.0, 18.0] out=[9.0, 9.0, 9.0]) (bins=9)</t>
         </is>
       </c>
     </row>
@@ -2812,29 +2812,29 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Brobdingnag</t>
+          <t>Atlantis</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C67" t="n">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="D67" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E67" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F67" t="n">
         <v>0</v>
       </c>
       <c r="G67" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H67" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I67" t="n">
         <v>0</v>
@@ -2846,17 +2846,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Dinotopia</t>
+          <t>Brobdingnag</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C68" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D68" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E68" t="n">
         <v>0</v>
@@ -2865,7 +2865,7 @@
         <v>0</v>
       </c>
       <c r="G68" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H68" t="n">
         <v>0</v>
@@ -2880,29 +2880,29 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Erewhon</t>
+          <t>Carpania</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C69" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D69" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F69" t="n">
         <v>0</v>
       </c>
       <c r="G69" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I69" t="n">
         <v>0</v>
@@ -2914,26 +2914,26 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Atlantis</t>
+          <t>Dinotopia</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C70" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="D70" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" t="n">
         <v>5</v>
-      </c>
-      <c r="F70" t="n">
-        <v>0</v>
-      </c>
-      <c r="G70" t="n">
-        <v>11</v>
       </c>
       <c r="H70" t="n">
         <v>0</v>
@@ -2948,17 +2948,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Carpania</t>
+          <t>Erewhon</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C71" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D71" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E71" t="n">
         <v>0</v>
@@ -2967,7 +2967,7 @@
         <v>0</v>
       </c>
       <c r="G71" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H71" t="n">
         <v>0</v>
@@ -2994,7 +2994,7 @@
         </is>
       </c>
       <c r="E73" t="n">
-        <v>1.192603901611535</v>
+        <v>0.1100783566303633</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -3003,7 +3003,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>alloy_transform (in=[2.0, 4.0] out=[2.0, 2.0, 2.0]) (bins=2)</t>
+          <t>alloy_transform (in=[10.0, 20.0] out=[10.0, 10.0, 10.0]) (bins=10)</t>
         </is>
       </c>
     </row>
@@ -3062,29 +3062,29 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Brobdingnag</t>
+          <t>Atlantis</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C75" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D75" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E75" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F75" t="n">
         <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H75" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I75" t="n">
         <v>0</v>
@@ -3096,17 +3096,17 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Dinotopia</t>
+          <t>Brobdingnag</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C76" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D76" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E76" t="n">
         <v>0</v>
@@ -3115,7 +3115,7 @@
         <v>0</v>
       </c>
       <c r="G76" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H76" t="n">
         <v>0</v>
@@ -3130,29 +3130,29 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Erewhon</t>
+          <t>Carpania</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C77" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D77" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F77" t="n">
         <v>0</v>
       </c>
       <c r="G77" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H77" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I77" t="n">
         <v>0</v>
@@ -3164,26 +3164,26 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Atlantis</t>
+          <t>Dinotopia</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C78" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="D78" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E78" t="n">
+        <v>0</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0</v>
+      </c>
+      <c r="G78" t="n">
         <v>5</v>
-      </c>
-      <c r="F78" t="n">
-        <v>0</v>
-      </c>
-      <c r="G78" t="n">
-        <v>11</v>
       </c>
       <c r="H78" t="n">
         <v>0</v>
@@ -3198,17 +3198,17 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Carpania</t>
+          <t>Erewhon</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C79" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D79" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E79" t="n">
         <v>0</v>
@@ -3217,7 +3217,7 @@
         <v>0</v>
       </c>
       <c r="G79" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H79" t="n">
         <v>0</v>

</xml_diff>